<commit_message>
changes to the structure
</commit_message>
<xml_diff>
--- a/Courses/Coursera courses co-ordinator_31 May 2020.xlsx
+++ b/Courses/Coursera courses co-ordinator_31 May 2020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monac\Documents\Training Courses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monac\Documents\Projects\-1.Study_and_Exploration\Courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A91B02-5E2A-45D1-9354-8BFDCE342FC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0484FA-153C-4B0B-B247-99B1339E67E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <t>Course name</t>
   </si>
@@ -206,12 +206,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M450"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +535,7 @@
     <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="87.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -551,28 +553,28 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="5"/>
+      <c r="L1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="6"/>
+      <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
@@ -604,7 +606,7 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="2">
@@ -613,7 +615,7 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="1">
         <v>43982</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -636,7 +638,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -648,7 +650,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -660,7 +662,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -672,7 +674,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -687,7 +689,7 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="2">
@@ -696,15 +698,12 @@
       <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="1">
         <v>43982</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
       <c r="G10" s="1">
         <v>43990</v>
       </c>
@@ -716,20 +715,20 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="2">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="2">
         <v>3</v>
       </c>
@@ -741,7 +740,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="2">
         <v>4</v>
       </c>
@@ -753,7 +752,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="2">
         <v>5</v>
       </c>
@@ -765,7 +764,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="2">
         <v>6</v>
       </c>
@@ -780,7 +779,7 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="2">
@@ -789,7 +788,7 @@
       <c r="C17" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="1">
         <v>43982</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -797,7 +796,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="2">
         <v>2</v>
       </c>
@@ -809,20 +808,20 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="2">
         <v>3</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="2">
         <v>4</v>
       </c>
@@ -834,7 +833,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="2">
         <v>5</v>
       </c>
@@ -849,7 +848,7 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="2">
@@ -858,7 +857,7 @@
       <c r="C23" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="1">
         <v>43982</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -866,7 +865,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="6"/>
       <c r="B24" s="2">
         <v>2</v>
       </c>
@@ -878,7 +877,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="2">
         <v>3</v>
       </c>
@@ -890,7 +889,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="6"/>
       <c r="B26" s="2">
         <v>4</v>
       </c>
@@ -919,7 +918,7 @@
       <c r="C29" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="1">
         <v>43982</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -933,7 +932,7 @@
       <c r="C30" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="1">
         <v>43982</v>
       </c>
       <c r="E30" s="4" t="s">
@@ -2244,7 +2243,7 @@
           <x14:formula1>
             <xm:f>'Validation support sheet'!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F4</xm:sqref>
+          <xm:sqref>F4:F207</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>